<commit_message>
oops + new features and capabilities
</commit_message>
<xml_diff>
--- a/etc/CONFIG.xlsx
+++ b/etc/CONFIG.xlsx
@@ -1,33 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TM\jatayu\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BE2454-89AB-499A-9C4D-A85683D44D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AE977B-10A9-4809-8506-3D9FE3CFC04D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PATHS" sheetId="2" r:id="rId1"/>
-    <sheet name="PROJECTS" sheetId="3" r:id="rId2"/>
-    <sheet name="ETC" sheetId="4" r:id="rId3"/>
+    <sheet name="TEMPVAR" sheetId="1" r:id="rId1"/>
+    <sheet name="PATHS" sheetId="2" r:id="rId2"/>
+    <sheet name="PROJECTS" sheetId="3" r:id="rId3"/>
+    <sheet name="ETC" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>ProjectPath</t>
-  </si>
-  <si>
-    <t>TestResultPath</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>C:\\Users\\asingh\\PycharmProjects\\Markdemo\\demo\\test_suite\PSE\5.PSELOGIN.xlsm</t>
+  </si>
+  <si>
+    <t>PSELOGIN_TestCase</t>
   </si>
   <si>
     <t>Projects</t>
@@ -36,19 +37,13 @@
     <t>RunY/N</t>
   </si>
   <si>
+    <t>TIME</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
-    <t>TIME</t>
-  </si>
-  <si>
-    <t>C:\\Users\</t>
-  </si>
-  <si>
     <t>PROJECT1</t>
-  </si>
-  <si>
-    <t>C:\\TM\\jatayu\\test_suite\\</t>
   </si>
   <si>
     <t>PROJECT2</t>
@@ -390,11 +385,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,33 +422,16 @@
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -447,18 +450,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -466,7 +469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -478,7 +481,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1">
         <v>4</v>

</xml_diff>